<commit_message>
add data, just finished nevada
</commit_message>
<xml_diff>
--- a/data/HouseOfRepresentatives.xlsx
+++ b/data/HouseOfRepresentatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessj\Documents\city tech\honors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8774405A-5D68-4FFF-AD82-178C15784222}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2857BCB-DDEF-49B2-89F1-77DD7E4DD048}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="15540" firstSheet="21" activeTab="24" xr2:uid="{692464C5-5044-4A4A-BAAD-F0B81373FE95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="15540" firstSheet="27" activeTab="30" xr2:uid="{692464C5-5044-4A4A-BAAD-F0B81373FE95}"/>
   </bookViews>
   <sheets>
     <sheet name="ALABAMA" sheetId="1" r:id="rId1"/>
@@ -38,14 +38,23 @@
     <sheet name="MARYLAND" sheetId="26" r:id="rId23"/>
     <sheet name="MASSACHUSETTS" sheetId="27" r:id="rId24"/>
     <sheet name="MICHIGAN" sheetId="28" r:id="rId25"/>
-    <sheet name="IDAHO (14)" sheetId="31" r:id="rId26"/>
-    <sheet name="IDAHO (13)" sheetId="30" r:id="rId27"/>
-    <sheet name="IDAHO (16)" sheetId="33" r:id="rId28"/>
-    <sheet name="IDAHO (12)" sheetId="29" r:id="rId29"/>
-    <sheet name="IDAHO (15)" sheetId="32" r:id="rId30"/>
+    <sheet name="MINNESOTA" sheetId="31" r:id="rId26"/>
+    <sheet name="MISSISSIPPI" sheetId="30" r:id="rId27"/>
+    <sheet name="MISSOURI" sheetId="33" r:id="rId28"/>
+    <sheet name="MONTANA" sheetId="29" r:id="rId29"/>
+    <sheet name="NEBRASKA" sheetId="32" r:id="rId30"/>
+    <sheet name="NEVADA" sheetId="43" r:id="rId31"/>
+    <sheet name="IDAHO (17)" sheetId="35" r:id="rId32"/>
+    <sheet name="IDAHO (18)" sheetId="36" r:id="rId33"/>
+    <sheet name="IDAHO (16)" sheetId="34" r:id="rId34"/>
+    <sheet name="IDAHO (19)" sheetId="37" r:id="rId35"/>
+    <sheet name="IDAHO (20)" sheetId="38" r:id="rId36"/>
+    <sheet name="IDAHO (24)" sheetId="42" r:id="rId37"/>
+    <sheet name="IDAHO (23)" sheetId="41" r:id="rId38"/>
+    <sheet name="IDAHO (21)" sheetId="39" r:id="rId39"/>
+    <sheet name="IDAHO (22)" sheetId="40" r:id="rId40"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -61,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3298" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="873">
   <si>
     <t>Year</t>
   </si>
@@ -2386,6 +2395,300 @@
   </si>
   <si>
     <t>Marcia Squier</t>
+  </si>
+  <si>
+    <t>Tim Walz</t>
+  </si>
+  <si>
+    <t>DFL</t>
+  </si>
+  <si>
+    <t>Jim Hagedorn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason Lewis </t>
+  </si>
+  <si>
+    <t>Angie Craig</t>
+  </si>
+  <si>
+    <t>Paula Overby</t>
+  </si>
+  <si>
+    <t>IDP</t>
+  </si>
+  <si>
+    <t>Erik Paulsen</t>
+  </si>
+  <si>
+    <t>Terri E. Bonoff</t>
+  </si>
+  <si>
+    <t>Betty McCollum</t>
+  </si>
+  <si>
+    <t>Greg Ryan</t>
+  </si>
+  <si>
+    <t>Susan Pendergast Sindt</t>
+  </si>
+  <si>
+    <t>LMN</t>
+  </si>
+  <si>
+    <t>Keith Ellison</t>
+  </si>
+  <si>
+    <t>Frank Nelson Drake</t>
+  </si>
+  <si>
+    <t>Dennis Schuller</t>
+  </si>
+  <si>
+    <t>Tom Emmer</t>
+  </si>
+  <si>
+    <t>David Synder</t>
+  </si>
+  <si>
+    <t>Collin Peterson</t>
+  </si>
+  <si>
+    <t>Dave Hughes</t>
+  </si>
+  <si>
+    <t>Rick Nolan</t>
+  </si>
+  <si>
+    <t>Stewart Mills</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trent Kelly </t>
+  </si>
+  <si>
+    <t>Jacob Owens</t>
+  </si>
+  <si>
+    <t>Chase Wilson</t>
+  </si>
+  <si>
+    <t>Cathy L. Toole</t>
+  </si>
+  <si>
+    <t>rEF</t>
+  </si>
+  <si>
+    <t>Bennie Thompson</t>
+  </si>
+  <si>
+    <t>John II Bouie</t>
+  </si>
+  <si>
+    <t>Troy Ray</t>
+  </si>
+  <si>
+    <t>Johnny McLeod</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>Gregg Harper</t>
+  </si>
+  <si>
+    <t>Dennis Quinn</t>
+  </si>
+  <si>
+    <t>Roger I. Gerrard</t>
+  </si>
+  <si>
+    <t>VPA</t>
+  </si>
+  <si>
+    <t>Lajena Sheets</t>
+  </si>
+  <si>
+    <t>Steven Palazzon</t>
+  </si>
+  <si>
+    <t>Mark Gladney</t>
+  </si>
+  <si>
+    <t>Richard Blake McCluskey</t>
+  </si>
+  <si>
+    <t>Shawn O'Hara</t>
+  </si>
+  <si>
+    <t>Lacy Clay</t>
+  </si>
+  <si>
+    <t>Steven G. Bailey</t>
+  </si>
+  <si>
+    <t>Robb E. Cunningham</t>
+  </si>
+  <si>
+    <t>Ann Wagner</t>
+  </si>
+  <si>
+    <t>Bill Otto</t>
+  </si>
+  <si>
+    <t>Jim Higgins</t>
+  </si>
+  <si>
+    <t>David Justus Arnold</t>
+  </si>
+  <si>
+    <t>Blaine Luetkemeyer</t>
+  </si>
+  <si>
+    <t>Kevin Miller</t>
+  </si>
+  <si>
+    <t>Dan Hogan</t>
+  </si>
+  <si>
+    <t>Doanita Simmons</t>
+  </si>
+  <si>
+    <t>Harold Davis</t>
+  </si>
+  <si>
+    <t>Vicky Hartzler</t>
+  </si>
+  <si>
+    <t>Gordon Christensen</t>
+  </si>
+  <si>
+    <t>Mark Bliss</t>
+  </si>
+  <si>
+    <t>Emmanuel II Cleaver</t>
+  </si>
+  <si>
+    <t>Jacob Turk</t>
+  </si>
+  <si>
+    <t>Roy Welborn</t>
+  </si>
+  <si>
+    <t>Sam Graves</t>
+  </si>
+  <si>
+    <t>David M. Blackwell</t>
+  </si>
+  <si>
+    <t>Russ Lee Monchil</t>
+  </si>
+  <si>
+    <t>Mike Diel</t>
+  </si>
+  <si>
+    <t>Billy Long</t>
+  </si>
+  <si>
+    <t>Genevieve (Gen) Williams</t>
+  </si>
+  <si>
+    <t>Benjamin T. Brixey</t>
+  </si>
+  <si>
+    <t>Amber Thomsen</t>
+  </si>
+  <si>
+    <t>Jason Smith</t>
+  </si>
+  <si>
+    <t>Dave Cowell</t>
+  </si>
+  <si>
+    <t>Jonathan Shell</t>
+  </si>
+  <si>
+    <t>Ryan Zinke</t>
+  </si>
+  <si>
+    <t>Denise Juneau</t>
+  </si>
+  <si>
+    <t>Rick Breckenridge</t>
+  </si>
+  <si>
+    <t>* chosen by the party to fill the vacany left by the death of Mike Fellows on the general election ballot</t>
+  </si>
+  <si>
+    <t>Jeff Fortenberry</t>
+  </si>
+  <si>
+    <t>Daniel M. Wik</t>
+  </si>
+  <si>
+    <t>Don Bacon</t>
+  </si>
+  <si>
+    <t>Brad Ashford</t>
+  </si>
+  <si>
+    <t>Steven Laird</t>
+  </si>
+  <si>
+    <t>Adrian Smith</t>
+  </si>
+  <si>
+    <t>Dina Titus</t>
+  </si>
+  <si>
+    <t>Mary Perry</t>
+  </si>
+  <si>
+    <t>Reuben D'Silva</t>
+  </si>
+  <si>
+    <t>NPY</t>
+  </si>
+  <si>
+    <t>Kamau A. Bakari</t>
+  </si>
+  <si>
+    <t>IAP</t>
+  </si>
+  <si>
+    <t>Mark E. Amodei</t>
+  </si>
+  <si>
+    <t>H. D (Chip) Evans</t>
+  </si>
+  <si>
+    <t>John H. Everhart</t>
+  </si>
+  <si>
+    <t>Drew Knight</t>
+  </si>
+  <si>
+    <t>Jacky Rosen</t>
+  </si>
+  <si>
+    <t>Danny Tarkanian</t>
+  </si>
+  <si>
+    <t>Warren Markowitz</t>
+  </si>
+  <si>
+    <t>David Goossen</t>
+  </si>
+  <si>
+    <t>Ruben Kihuen</t>
+  </si>
+  <si>
+    <t>Cresent Hardy</t>
+  </si>
+  <si>
+    <t>Steve Brown</t>
+  </si>
+  <si>
+    <t>Mike Little</t>
   </si>
 </sst>
 </file>
@@ -19629,7 +19932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AACA7C7C-FBB3-43CC-A58D-D8C159901A8B}">
   <dimension ref="A1:J78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
@@ -21063,8 +21366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E6E4DA-6B3E-46EB-9F01-38F87CCC248E}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21115,13 +21418,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>775</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>776</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>169074</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -21135,13 +21438,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>777</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>166526</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -21155,13 +21458,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>598</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>277</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -21172,19 +21475,19 @@
         <v>2016</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>778</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>173970</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -21192,16 +21495,16 @@
         <v>2016</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>779</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>776</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>167315</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -21209,41 +21512,504 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="F7" s="4">
+        <v>28869</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4">
+        <v>360</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
+        <v>223077</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F10" s="4">
+        <v>169243</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1144</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F12" s="4">
+        <v>203299</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="4">
+        <v>121032</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="F14" s="4">
+        <v>27152</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="4">
+        <v>461</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F16" s="4">
+        <v>249964</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4">
+        <v>80660</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>787</v>
+      </c>
+      <c r="F18" s="4">
+        <v>30759</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="4">
+        <v>499</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C20" s="4">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4">
+        <v>235380</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="4">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F21" s="4">
+        <v>123008</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="4">
+        <v>536</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C23" s="4">
+        <v>7</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F23" s="4">
+        <v>173589</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="4">
+        <v>156952</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C25" s="4">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="4">
+        <v>307</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C26" s="4">
+        <v>8</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>776</v>
+      </c>
+      <c r="F26" s="4">
+        <v>179098</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C27" s="4">
+        <v>8</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" s="4">
+        <v>177089</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="4">
+        <v>792</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
         <v>2014</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
+      <c r="B35" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="4">
+        <v>2014</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <v>2014</v>
+      </c>
       <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="4">
+        <v>2014</v>
+      </c>
       <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -21303,8 +22069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE7ECD6-97D0-4F85-87E4-B14B18D475B7}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21355,13 +22121,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>797</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>206455</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -21375,13 +22141,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>798</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>83947</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -21395,13 +22161,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>799</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>6181</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -21415,13 +22181,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>800</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>801</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>3840</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>14</v>
@@ -21432,48 +22198,323 @@
         <v>2016</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>802</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>192343</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4">
+        <v>83541</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="4">
+        <v>6918</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3823</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="4">
+        <v>209490</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4">
+        <v>96101</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>810</v>
+      </c>
+      <c r="F12" s="4">
+        <v>8696</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2158</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>181323</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4">
+        <v>77505</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="4">
+        <v>14687</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>815</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>806</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5264</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
         <v>2014</v>
       </c>
     </row>
@@ -21543,8 +22584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE6DAA00-C4CD-40C9-B8D6-23D0489641EF}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21595,13 +22636,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>816</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>236993</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -21615,13 +22656,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>817</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>62714</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -21635,13 +22676,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>818</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>14317</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -21652,19 +22693,19 @@
         <v>2016</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>819</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>241954</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -21672,16 +22713,16 @@
         <v>2016</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>820</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>155689</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -21689,36 +22730,521 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="4">
+        <v>11758</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3895</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
+        <v>249865</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>824</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>102891</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>825</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F11" s="4">
+        <v>11962</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="F12" s="4">
+        <v>3605</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>827</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4">
+        <v>10</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>828</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>225348</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4">
+        <v>92510</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="4">
+        <v>14376</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>831</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="4">
+        <v>190766</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4">
+        <v>123771</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>833</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9733</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C20" s="4">
+        <v>6</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>834</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="4">
+        <v>238388</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="4">
+        <v>6</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="4">
+        <v>99692</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C22" s="4">
+        <v>6</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>836</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F22" s="4">
+        <v>8123</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C23" s="4">
+        <v>6</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>837</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4241</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="4">
+        <v>228692</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C25" s="4">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>839</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="4">
+        <v>92756</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C26" s="4">
+        <v>7</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F26" s="4">
+        <v>17153</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C27" s="4">
+        <v>7</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="4">
+        <v>6</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>842</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="4">
+        <v>229792</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C29" s="4">
+        <v>8</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>843</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="4">
+        <v>70009</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C30" s="4">
+        <v>8</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>844</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30" s="4">
+        <v>9070</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
+      <c r="B35" s="4">
+        <v>2014</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H37" s="4"/>
@@ -21783,8 +23309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB72462E-79DB-4E4B-91BF-570A02DEFF66}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21835,13 +23361,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>845</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>285358</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -21855,19 +23381,19 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>846</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>205919</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="4">
         <v>2016</v>
       </c>
@@ -21875,53 +23401,32 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>847</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>16554</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="4">
-        <v>2016</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4">
-        <v>181</v>
+        <v>2014</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" s="4">
-        <v>2016</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4">
-        <v>171</v>
+        <v>2014</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -21929,31 +23434,6 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B12" s="4">
         <v>2014</v>
       </c>
     </row>
@@ -22263,6 +23743,2458 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{342BC384-924C-4BF2-BD22-1870FA3BBF10}">
   <dimension ref="A1:J54"/>
   <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>189771</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>83467</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="4">
+        <v>141066</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>137602</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>853</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="4">
+        <v>9640</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>854</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4">
+        <v>226720</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCE8D88-85EB-4DBD-A0A7-5630F5FE276F}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4">
+        <v>116537</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>856</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4">
+        <v>54174</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>857</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="F4" s="4">
+        <v>13897</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>859</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3744</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <v>182676</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>862</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4">
+        <v>115722</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>863</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8693</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="F9" s="4">
+        <v>6245</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>146869</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>866</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>142926</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>3</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>867</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F12" s="4">
+        <v>11602</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>868</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>858</v>
+      </c>
+      <c r="F13" s="4">
+        <v>9566</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>4</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>869</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="4">
+        <v>128985</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>4</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>870</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="4">
+        <v>118328</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>871</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F16" s="4">
+        <v>10206</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>872</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>860</v>
+      </c>
+      <c r="F17" s="4">
+        <v>8327</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE16EE-3A9F-4B6B-8AFC-E9A2B6D14B2C}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11E0670-81C9-437F-B612-F81BAFE60BE4}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1BED6B-5282-4184-834B-D088CCD0707F}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EC84CD-FEFF-4476-B38D-FC36DA7D6535}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F5E3773-810F-454F-A59E-001EA7BCFAA6}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D718F7FE-C374-4440-BAEC-AC2DE916F806}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7F314A3-CDAB-42FE-B3ED-574C53631D27}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B6EF183-3D66-4670-9541-2C5F5A4D48D9}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
@@ -26784,6 +30716,246 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349CC5E9-CBF4-47C4-B68F-6CAD2C3DB02E}">
+  <dimension ref="A1:J54"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="8.7265625" style="4"/>
+    <col min="4" max="4" width="43.7265625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="34.81640625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="17.54296875" style="4" customWidth="1"/>
+    <col min="8" max="9" width="61" style="6" customWidth="1"/>
+    <col min="10" max="10" width="65.54296875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B2" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="4">
+        <v>8923</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1581</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4">
+        <v>978</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4">
+        <v>181</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="4">
+        <v>171</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H37" s="4"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H38" s="4"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H39" s="4"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="4"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE7EA3D4-69EE-4A03-9582-DD2886CB999C}">
   <dimension ref="A1:J54"/>

</xml_diff>

<commit_message>
add more data, up to 2016 new york district 6
</commit_message>
<xml_diff>
--- a/data/HouseOfRepresentatives.xlsx
+++ b/data/HouseOfRepresentatives.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessj\Documents\city tech\honors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2857BCB-DDEF-49B2-89F1-77DD7E4DD048}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD5F85F-6222-40B7-99BF-4CE5AE3E0639}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="15540" firstSheet="27" activeTab="30" xr2:uid="{692464C5-5044-4A4A-BAAD-F0B81373FE95}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27360" windowHeight="15540" firstSheet="27" activeTab="34" xr2:uid="{692464C5-5044-4A4A-BAAD-F0B81373FE95}"/>
   </bookViews>
   <sheets>
     <sheet name="ALABAMA" sheetId="1" r:id="rId1"/>
@@ -44,10 +44,10 @@
     <sheet name="MONTANA" sheetId="29" r:id="rId29"/>
     <sheet name="NEBRASKA" sheetId="32" r:id="rId30"/>
     <sheet name="NEVADA" sheetId="43" r:id="rId31"/>
-    <sheet name="IDAHO (17)" sheetId="35" r:id="rId32"/>
-    <sheet name="IDAHO (18)" sheetId="36" r:id="rId33"/>
-    <sheet name="IDAHO (16)" sheetId="34" r:id="rId34"/>
-    <sheet name="IDAHO (19)" sheetId="37" r:id="rId35"/>
+    <sheet name="NEW HAMPSHIRE" sheetId="35" r:id="rId32"/>
+    <sheet name="NEW JERSEY" sheetId="36" r:id="rId33"/>
+    <sheet name="NEW MEXICO" sheetId="34" r:id="rId34"/>
+    <sheet name="NEW YORK" sheetId="37" r:id="rId35"/>
     <sheet name="IDAHO (20)" sheetId="38" r:id="rId36"/>
     <sheet name="IDAHO (24)" sheetId="42" r:id="rId37"/>
     <sheet name="IDAHO (23)" sheetId="41" r:id="rId38"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4012" uniqueCount="985">
   <si>
     <t>Year</t>
   </si>
@@ -2689,6 +2689,342 @@
   </si>
   <si>
     <t>Mike Little</t>
+  </si>
+  <si>
+    <t>Carol Shea-Porter</t>
+  </si>
+  <si>
+    <t>Frank Guinta</t>
+  </si>
+  <si>
+    <t>Rich Ashooh</t>
+  </si>
+  <si>
+    <t>Shawn P. O'Connor</t>
+  </si>
+  <si>
+    <t>Brendan Kelly</t>
+  </si>
+  <si>
+    <t>Robert Lombardo</t>
+  </si>
+  <si>
+    <t>John Potucek</t>
+  </si>
+  <si>
+    <t>Ann McLane Kuster</t>
+  </si>
+  <si>
+    <t>Jim Lawrence</t>
+  </si>
+  <si>
+    <t>John J. Babiarz</t>
+  </si>
+  <si>
+    <t>Donald W. Norcross</t>
+  </si>
+  <si>
+    <t>Bob Patterson</t>
+  </si>
+  <si>
+    <t>Scot John Tomaszewski</t>
+  </si>
+  <si>
+    <t>WDB</t>
+  </si>
+  <si>
+    <t>William F. IV Sihr</t>
+  </si>
+  <si>
+    <t>Michael Berman</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>Frank A. LoBiondo</t>
+  </si>
+  <si>
+    <t>David H. Cole</t>
+  </si>
+  <si>
+    <t>John Ordille</t>
+  </si>
+  <si>
+    <t>James Keenan</t>
+  </si>
+  <si>
+    <t>MGW</t>
+  </si>
+  <si>
+    <t>Steven Fenichel</t>
+  </si>
+  <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>Eric Beechwood</t>
+  </si>
+  <si>
+    <t>PIP</t>
+  </si>
+  <si>
+    <t>Gabriel Brian Franco</t>
+  </si>
+  <si>
+    <t>FPR</t>
+  </si>
+  <si>
+    <t>Tom MacArthur</t>
+  </si>
+  <si>
+    <t>Frederick John LaVergne</t>
+  </si>
+  <si>
+    <t>Lawrence W. Jr. Berlinski</t>
+  </si>
+  <si>
+    <t>Christopher H. Smith</t>
+  </si>
+  <si>
+    <t>Lorna Phillipson</t>
+  </si>
+  <si>
+    <t>Hank Schroeder</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>Jeremy Marcus</t>
+  </si>
+  <si>
+    <t>Joshua S. Gottheimer</t>
+  </si>
+  <si>
+    <t>Scott Garrett</t>
+  </si>
+  <si>
+    <t>Claudio Belusic</t>
+  </si>
+  <si>
+    <t>Frank Jr. Pallone</t>
+  </si>
+  <si>
+    <t>Brent Sonnek-Schmelz</t>
+  </si>
+  <si>
+    <t>Rajit B. Malliah</t>
+  </si>
+  <si>
+    <t>Judith Shamy</t>
+  </si>
+  <si>
+    <t>Leonard Lance</t>
+  </si>
+  <si>
+    <t>Peter Jacob</t>
+  </si>
+  <si>
+    <t>Dan O'Neill</t>
+  </si>
+  <si>
+    <t>Arthurt T. Jr. Haussman</t>
+  </si>
+  <si>
+    <t>Albio Sires</t>
+  </si>
+  <si>
+    <t>Agha Khan</t>
+  </si>
+  <si>
+    <t>Pablo Olivera</t>
+  </si>
+  <si>
+    <t>WUA</t>
+  </si>
+  <si>
+    <t>Dan Delaney</t>
+  </si>
+  <si>
+    <t>Bill Jr. Pascrell</t>
+  </si>
+  <si>
+    <t>Hector L. Castillo</t>
+  </si>
+  <si>
+    <t>Diego Rivera</t>
+  </si>
+  <si>
+    <t>Jeff Boss</t>
+  </si>
+  <si>
+    <t>NSA</t>
+  </si>
+  <si>
+    <t>Donald M. Jr. Payne</t>
+  </si>
+  <si>
+    <t>David H. Pinckney</t>
+  </si>
+  <si>
+    <t>Joanne Miller</t>
+  </si>
+  <si>
+    <t>WOP</t>
+  </si>
+  <si>
+    <t>Aaron Walter Fraser</t>
+  </si>
+  <si>
+    <t>NBP</t>
+  </si>
+  <si>
+    <t>Rodney P. Frelinghuysen</t>
+  </si>
+  <si>
+    <t>Joseph M. Wenzel</t>
+  </si>
+  <si>
+    <t>Thomas Depasquale</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>Jeff Hetrick</t>
+  </si>
+  <si>
+    <t>Bonnie Watson Coleman</t>
+  </si>
+  <si>
+    <t>Steven J. Uccio</t>
+  </si>
+  <si>
+    <t>R. Edward Forchion</t>
+  </si>
+  <si>
+    <t>LMP</t>
+  </si>
+  <si>
+    <t>Robert Shapiro</t>
+  </si>
+  <si>
+    <t>TED</t>
+  </si>
+  <si>
+    <t>Thomas Fitzpatrick</t>
+  </si>
+  <si>
+    <t>Steven Welzer</t>
+  </si>
+  <si>
+    <t>Michael R. Bollentin</t>
+  </si>
+  <si>
+    <t>WTP</t>
+  </si>
+  <si>
+    <t>Michelle Lujan Grisham</t>
+  </si>
+  <si>
+    <t>Richard Gregory Priem</t>
+  </si>
+  <si>
+    <t>Steve Pearce</t>
+  </si>
+  <si>
+    <t>Merrie Lee Soules</t>
+  </si>
+  <si>
+    <t>Jack A. McGrann</t>
+  </si>
+  <si>
+    <t>Ben R. Lujan</t>
+  </si>
+  <si>
+    <t>Michael H. Romero</t>
+  </si>
+  <si>
+    <t>Lee M. Zeldin</t>
+  </si>
+  <si>
+    <t>Republican,CRV,REF,IDP</t>
+  </si>
+  <si>
+    <t>158409-23327-843-5920</t>
+  </si>
+  <si>
+    <t>Anna E. Throne-Holst</t>
+  </si>
+  <si>
+    <t>Democratic,WEP,WF</t>
+  </si>
+  <si>
+    <t>126635-2496-6147</t>
+  </si>
+  <si>
+    <t>Peter T. King</t>
+  </si>
+  <si>
+    <t>R/TRP,CRV,REF</t>
+  </si>
+  <si>
+    <t>157571-21810-2125</t>
+  </si>
+  <si>
+    <t>Du Wayne Gregory</t>
+  </si>
+  <si>
+    <t>Democratic,IDP,WEP,WF</t>
+  </si>
+  <si>
+    <t>102270-3213-1438-4017</t>
+  </si>
+  <si>
+    <t>Thomas R. Suozzi</t>
+  </si>
+  <si>
+    <t>Jack M. Martins</t>
+  </si>
+  <si>
+    <t>Republican,REF,CRV</t>
+  </si>
+  <si>
+    <t>133954-1940-16410</t>
+  </si>
+  <si>
+    <t>Kathleen M. Rice</t>
+  </si>
+  <si>
+    <t>181861-4562</t>
+  </si>
+  <si>
+    <t>David H. Gurfein</t>
+  </si>
+  <si>
+    <t>111246-14137-1055</t>
+  </si>
+  <si>
+    <t>Gregory W. Meeks</t>
+  </si>
+  <si>
+    <t>Democratic,WEP</t>
+  </si>
+  <si>
+    <t>197852-1963</t>
+  </si>
+  <si>
+    <t>Frank Francois</t>
+  </si>
+  <si>
+    <t>Michael A. O'Reilly</t>
+  </si>
+  <si>
+    <t>26791-3521</t>
+  </si>
+  <si>
+    <t>Republican,CRV</t>
   </si>
 </sst>
 </file>
@@ -23998,7 +24334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DCE8D88-85EB-4DBD-A0A7-5630F5FE276F}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -24515,8 +24851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE16EE-3A9F-4B6B-8AFC-E9A2B6D14B2C}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B33" sqref="A33:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24567,13 +24903,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>873</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>162080</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -24587,13 +24923,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>874</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>157176</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -24607,13 +24943,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>875</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>388</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>55</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -24627,13 +24963,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>876</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>34735</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>14</v>
@@ -24647,13 +24983,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>877</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>6074</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -24661,71 +24997,316 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F7" s="4">
+        <v>5507</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="4">
+        <v>194</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>879</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="4">
+        <v>163</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4">
+        <v>174495</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>158973</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>882</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="4">
+        <v>17088</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4">
+        <v>237</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.35">
@@ -24753,10 +25334,10 @@
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C11E0670-81C9-437F-B612-F81BAFE60BE4}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24807,13 +25388,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>883</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>183231</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -24827,13 +25408,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>884</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>112388</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -24847,13 +25428,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>885</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>886</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>5473</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -24867,13 +25448,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>887</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
+        <v>183</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>2410</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>14</v>
@@ -24887,13 +25468,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>888</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>889</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>1971</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -24901,90 +25482,1078 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>890</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="4">
+        <v>176338</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>891</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4">
+        <v>110838</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F9" s="4">
+        <v>3773</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>2</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>894</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2653</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>896</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1574</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>897</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>898</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1387</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>899</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1232</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>3</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>194596</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>902</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="4">
+        <v>127526</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>3</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="F16" s="4">
+        <v>5938</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="4">
+        <v>211992</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="4">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="4">
+        <v>11532</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>907</v>
+      </c>
+      <c r="F19" s="4">
+        <v>5840</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F20" s="4">
+        <v>3320</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C21" s="4">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>909</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="4">
+        <v>172587</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>910</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="4">
+        <v>157690</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F23" s="4">
+        <v>7424</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C24" s="4">
+        <v>6</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4">
+        <v>167895</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C25" s="4">
+        <v>6</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>913</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" s="4">
+        <v>91908</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C26" s="4">
+        <v>6</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>914</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F26" s="4">
+        <v>1912</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C27" s="4">
+        <v>6</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F27" s="4">
+        <v>1720</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C28" s="4">
+        <v>7</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="4">
+        <v>185850</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C29" s="4">
+        <v>7</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="4">
+        <v>148188</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C30" s="4">
+        <v>7</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>918</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30" s="4">
+        <v>5343</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C31" s="4">
+        <v>7</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>919</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="F31" s="4">
+        <v>4254</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C32" s="4">
+        <v>8</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>920</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="4">
+        <v>134733</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C33" s="4">
+        <v>8</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>921</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="4">
+        <v>32337</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C34" s="4">
+        <v>8</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>922</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="F34" s="4">
+        <v>4381</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C35" s="4">
+        <v>8</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>924</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F35" s="4">
+        <v>3438</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C36" s="4">
+        <v>9</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>925</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="4">
+        <v>162642</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C37" s="4">
+        <v>9</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>926</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" s="4">
+        <v>65376</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C38" s="4">
+        <v>9</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>927</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" s="4">
+        <v>3327</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C39" s="4">
+        <v>9</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>928</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1897</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C40" s="4">
+        <v>10</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>930</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="4">
+        <v>190856</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C41" s="4">
+        <v>10</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>931</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="4">
+        <v>26450</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C42" s="4">
+        <v>10</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>932</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>933</v>
+      </c>
+      <c r="F42" s="4">
+        <v>3719</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C43" s="4">
+        <v>10</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>934</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>935</v>
+      </c>
+      <c r="F43" s="4">
+        <v>1746</v>
+      </c>
+      <c r="G43" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C44" s="4">
+        <v>11</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>936</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="4">
+        <v>194299</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C45" s="4">
+        <v>11</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>937</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="4">
+        <v>130162</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C46" s="4">
+        <v>11</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>938</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>939</v>
+      </c>
+      <c r="F46" s="4">
+        <v>7056</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C47" s="4">
+        <v>11</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>940</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F47" s="4">
+        <v>3475</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C48" s="4">
+        <v>12</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>941</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="4">
+        <v>181430</v>
+      </c>
+      <c r="G48" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="H48" s="4"/>
     </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C49" s="4">
+        <v>12</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" s="4">
+        <v>92407</v>
+      </c>
+      <c r="G49" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C50" s="4">
+        <v>12</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>943</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>944</v>
+      </c>
+      <c r="F50" s="4">
+        <v>6094</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H50" s="4"/>
     </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B51" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C51" s="4">
+        <v>12</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>946</v>
+      </c>
+      <c r="F51" s="4">
+        <v>2775</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H51" s="4"/>
     </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B52" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C52" s="4">
+        <v>12</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F52" s="4">
+        <v>2482</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H52" s="4"/>
     </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C53" s="4">
+        <v>12</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2135</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H53" s="4"/>
     </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C54" s="4">
+        <v>12</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>949</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>950</v>
+      </c>
+      <c r="F54" s="4">
+        <v>1311</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G55" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G57" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G58" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B60" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B61" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B62" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B63" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B65" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B66" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B67" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B68" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B69" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B70" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B71" s="4">
+        <v>2014</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24995,8 +26564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1BED6B-5282-4184-834B-D088CCD0707F}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25047,13 +26616,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>951</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" s="4">
-        <v>8923</v>
+        <v>181088</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -25067,13 +26636,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>952</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F3" s="4">
-        <v>1581</v>
+        <v>96879</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -25084,19 +26653,19 @@
         <v>2016</v>
       </c>
       <c r="C4" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>953</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>143515</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -25104,16 +26673,16 @@
         <v>2016</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>954</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F5" s="4">
-        <v>181</v>
+        <v>85232</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>14</v>
@@ -25124,16 +26693,16 @@
         <v>2016</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>955</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="F6" s="4">
-        <v>171</v>
+        <v>70</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -25141,31 +26710,88 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>956</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4">
+        <v>170612</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>957</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="4">
+        <v>102730</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
         <v>2014</v>
       </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
         <v>2014</v>
       </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
         <v>2014</v>
       </c>
+      <c r="G11" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
+        <v>2014</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
         <v>2014</v>
       </c>
     </row>
@@ -25235,8 +26861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5EC84CD-FEFF-4476-B38D-FC36DA7D6535}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25287,13 +26913,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>186</v>
+        <v>958</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4">
-        <v>8923</v>
+        <v>959</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>960</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>10</v>
@@ -25307,13 +26933,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>961</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="4">
-        <v>1581</v>
+        <v>962</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>963</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>14</v>
@@ -25327,13 +26953,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>188</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F4" s="4">
-        <v>978</v>
+        <v>113</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>14</v>
@@ -25344,16 +26970,16 @@
         <v>2016</v>
       </c>
       <c r="C5" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>189</v>
+        <v>964</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="4">
-        <v>181</v>
+        <v>965</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>966</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>14</v>
@@ -25364,16 +26990,16 @@
         <v>2016</v>
       </c>
       <c r="C6" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>190</v>
+        <v>967</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="4">
-        <v>171</v>
+        <v>968</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>969</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>14</v>
@@ -25381,71 +27007,419 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4">
+        <v>151</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>970</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4">
+        <v>171775</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C9" s="4">
+        <v>3</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>971</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>972</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>973</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="4">
+        <v>175</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" s="4">
-        <v>2014</v>
+        <v>2016</v>
+      </c>
+      <c r="C11" s="4">
+        <v>4</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>974</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>962</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>975</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" s="4">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>2016</v>
+      </c>
+      <c r="C12" s="4">
+        <v>4</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>965</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>977</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4">
+        <v>139</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>978</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>979</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>980</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>982</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>983</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3587</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="4">
+        <v>2016</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4">
+        <v>139</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B37" s="4">
+        <v>2016</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="4">
+        <v>2016</v>
+      </c>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H42" s="4"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H43" s="4"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H44" s="4"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H45" s="4"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H46" s="4"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H47" s="4"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="H48" s="4"/>
     </row>
     <row r="49" spans="8:8" x14ac:dyDescent="0.35">

</xml_diff>